<commit_message>
added updated TGP data analysis slideshow
</commit_message>
<xml_diff>
--- a/data/ET_data.xlsx
+++ b/data/ET_data.xlsx
@@ -577,14 +577,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="14" max="14" width="29.33203125" customWidth="1"/>
-    <col min="26" max="26" width="12" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" customWidth="1"/>
+    <col min="11" max="11" width="23" customWidth="1"/>
+    <col min="14" max="14" width="12" customWidth="1"/>
+    <col min="26" max="26" width="40.1640625" customWidth="1"/>
+    <col min="38" max="38" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.2">

</xml_diff>